<commit_message>
Enlever l'entête du tableau
</commit_message>
<xml_diff>
--- a/SKINNER.xlsx
+++ b/SKINNER.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
   <si>
     <t>DESIGNATION</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>RIFF 2A+2B : VERY SLOW</t>
-  </si>
-  <si>
-    <t>BLAST</t>
   </si>
   <si>
     <t>X</t>
@@ -569,6 +566,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -578,18 +623,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -597,42 +630,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -939,7 +936,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,498 +953,496 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="13">
         <v>220</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="10"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="7"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24">
-        <v>8</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="18">
+        <v>8</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="18">
         <v>220</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="26"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="20"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="24">
-        <v>8</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="18">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="18">
         <v>220</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="26"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="20"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="24">
-        <v>8</v>
-      </c>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="18">
+        <v>8</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="18">
         <v>220</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="26"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="20"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="24">
-        <v>8</v>
-      </c>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="18">
+        <v>8</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="18">
         <v>190</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="26"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="20"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="24">
-        <v>8</v>
-      </c>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="18">
+        <v>8</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="18">
         <v>190</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="26"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="20"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="24">
-        <v>8</v>
-      </c>
-      <c r="C10" s="25" t="s">
+      <c r="A10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18">
+        <v>8</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="18">
         <v>190</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="26"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="20"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="24">
-        <v>8</v>
-      </c>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="18">
+        <v>8</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="18">
         <v>190</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="26"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="20"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="24">
-        <v>8</v>
-      </c>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="18">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="18">
         <v>190</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="26"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="20"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="24">
-        <v>8</v>
-      </c>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="18">
+        <v>8</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="18">
         <v>190</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="26"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="20"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="24">
-        <v>8</v>
-      </c>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="18">
+        <v>8</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="18">
         <v>190</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="26"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="20"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="24">
-        <v>8</v>
-      </c>
-      <c r="C15" s="25" t="s">
+      <c r="B15" s="18">
+        <v>8</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="18">
         <v>190</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="26"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="20"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="24">
-        <v>8</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="18">
+        <v>8</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="18">
         <v>190</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="26"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="20"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="24">
-        <v>8</v>
-      </c>
-      <c r="C17" s="25" t="s">
+      <c r="B17" s="18">
+        <v>8</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="18">
         <v>190</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="26"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="20"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="24">
-        <v>8</v>
-      </c>
-      <c r="C18" s="25" t="s">
+      <c r="B18" s="18">
+        <v>8</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="18">
         <v>190</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="26"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="20"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="24">
-        <v>8</v>
-      </c>
-      <c r="C19" s="25" t="s">
+      <c r="B19" s="18">
+        <v>8</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="18">
         <v>190</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="26"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="20"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="15">
         <v>16</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="15">
         <v>190</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="12"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="9"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1530,472 +1525,472 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="17" t="s">
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B4" s="13">
+        <v>8</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="13">
+        <v>175</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="19">
-        <v>8</v>
-      </c>
-      <c r="C4" s="20" t="s">
+      <c r="B5" s="18">
+        <v>8</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D5" s="18">
         <v>175</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="24">
-        <v>8</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B6" s="18">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D6" s="18">
         <v>175</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="24">
-        <v>8</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B7" s="18">
+        <v>12</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="18">
+        <v>175</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="18">
+        <v>16</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D8" s="18">
         <v>175</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="24">
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="18">
         <v>12</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="24">
+      <c r="C9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="18">
         <v>175</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="24">
-        <v>16</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="24">
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="18">
+        <v>4</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="18">
         <v>175</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="24">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="18">
+        <v>175</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="18">
+        <v>175</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="18">
         <v>12</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="24">
+      <c r="C13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="18">
         <v>175</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="24">
-        <v>4</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="24">
+      <c r="E13" s="18"/>
+      <c r="F13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="18">
+        <v>8</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="18">
         <v>175</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="24"/>
-      <c r="I10" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="24">
-        <v>2</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="24">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="18">
+        <v>8</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="18">
         <v>175</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="24">
-        <v>2</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="24">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="18">
+        <v>8</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="18">
         <v>175</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="24">
-        <v>12</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="24">
+      <c r="E16" s="18"/>
+      <c r="F16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="18">
+        <v>8</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="18">
         <v>175</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="24">
-        <v>8</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="24">
+      <c r="E17" s="18"/>
+      <c r="F17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="18">
+        <v>8</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="18">
         <v>175</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="24">
-        <v>8</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="24">
-        <v>175</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="24">
-        <v>8</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="24">
-        <v>175</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="24">
-        <v>8</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="24">
-        <v>175</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="24">
-        <v>8</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="24">
-        <v>175</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="26" t="s">
-        <v>33</v>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="26"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="12"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>